<commit_message>
Fixed the single element issue
For one of the website the entries are parsed  as single entry. Splitted it by \n and working. But still if the jobs are same name, then it is not detected.
</commit_message>
<xml_diff>
--- a/JobAlert - Copy.xlsx
+++ b/JobAlert - Copy.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learn\Projects\Focux\Focux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{B193496D-B143-45D3-B9FD-E48CAAF56015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD733941-59D1-4A10-9CD1-EF45DCC73E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Index</t>
   </si>
@@ -81,12 +81,39 @@
   </si>
   <si>
     <t>Job_CSS_Sel</t>
+  </si>
+  <si>
+    <t>//*[@id="usercentrics-root"]</t>
+  </si>
+  <si>
+    <t>data-testid="uc-accept-all-button"</t>
+  </si>
+  <si>
+    <t>class="item-title"</t>
+  </si>
+  <si>
+    <t>/html/body/header/dock-privacy-settings</t>
+  </si>
+  <si>
+    <t>class="a-button a-button--primary -without-icon"</t>
+  </si>
+  <si>
+    <t>class="A-JobPanel__title"</t>
+  </si>
+  <si>
+    <t>LoadTime_s</t>
+  </si>
+  <si>
+    <t>class="css-qiqmbt"</t>
+  </si>
+  <si>
+    <t>id="JOBRESULTLIST--jobList"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -125,12 +152,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -466,22 +492,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
     <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" customWidth="1"/>
     <col min="6" max="6" width="10.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -491,7 +516,7 @@
       <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>10</v>
       </c>
       <c r="D1" t="s">
@@ -504,10 +529,10 @@
         <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -517,8 +542,17 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -528,8 +562,17 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -542,6 +585,9 @@
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -550,16 +596,22 @@
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C5" r:id="rId3" location="/SEARCH/SIMPLE/"/>
-    <hyperlink ref="C4" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{194CCAA1-18FD-445C-A039-7AB48874E9B7}"/>
+    <hyperlink ref="C5" r:id="rId2" location="/SEARCH/SIMPLE/" xr:uid="{EF58474E-0777-40D2-9489-DCB1B0F51131}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{632E38C5-EA31-4409-94BA-AD6FB102AB52}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{8D2150E3-0FF3-40A4-B80C-9EBD646D1831}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>